<commit_message>
update rekursiv and updated data file
</commit_message>
<xml_diff>
--- a/Keyword_Analysis.xlsx
+++ b/Keyword_Analysis.xlsx
@@ -668,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -756,7 +756,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -822,7 +822,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -899,7 +899,7 @@
         <v>9</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -987,7 +987,7 @@
         <v>9</v>
       </c>
       <c r="C31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -998,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1009,7 +1009,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1383,7 +1383,7 @@
         <v>5</v>
       </c>
       <c r="C67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1438,7 +1438,7 @@
         <v>10</v>
       </c>
       <c r="C72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -1493,7 +1493,7 @@
         <v>7</v>
       </c>
       <c r="C77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1625,7 +1625,7 @@
         <v>11</v>
       </c>
       <c r="C89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -1724,7 +1724,7 @@
         <v>4</v>
       </c>
       <c r="C98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -2252,7 +2252,7 @@
         <v>4</v>
       </c>
       <c r="C146" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -2494,7 +2494,7 @@
         <v>10</v>
       </c>
       <c r="C168" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -2505,7 +2505,7 @@
         <v>11</v>
       </c>
       <c r="C169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -2516,7 +2516,7 @@
         <v>4</v>
       </c>
       <c r="C170" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
@@ -2582,7 +2582,7 @@
         <v>10</v>
       </c>
       <c r="C176" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -2615,7 +2615,7 @@
         <v>5</v>
       </c>
       <c r="C179" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -2648,7 +2648,7 @@
         <v>8</v>
       </c>
       <c r="C182" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -2692,7 +2692,7 @@
         <v>4</v>
       </c>
       <c r="C186" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -2714,7 +2714,7 @@
         <v>6</v>
       </c>
       <c r="C188" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -2725,7 +2725,7 @@
         <v>7</v>
       </c>
       <c r="C189" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -2736,7 +2736,7 @@
         <v>8</v>
       </c>
       <c r="C190" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -2780,7 +2780,7 @@
         <v>4</v>
       </c>
       <c r="C194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
@@ -2813,7 +2813,7 @@
         <v>7</v>
       </c>
       <c r="C197" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
@@ -2824,7 +2824,7 @@
         <v>8</v>
       </c>
       <c r="C198" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
@@ -2912,7 +2912,7 @@
         <v>8</v>
       </c>
       <c r="C206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -3396,7 +3396,7 @@
         <v>4</v>
       </c>
       <c r="C250" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
@@ -3462,7 +3462,7 @@
         <v>10</v>
       </c>
       <c r="C256" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
@@ -3550,7 +3550,7 @@
         <v>10</v>
       </c>
       <c r="C264" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265">
@@ -3825,7 +3825,7 @@
         <v>11</v>
       </c>
       <c r="C289" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290">
@@ -4067,7 +4067,7 @@
         <v>9</v>
       </c>
       <c r="C311" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312">
@@ -4078,7 +4078,7 @@
         <v>10</v>
       </c>
       <c r="C312" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="313">
@@ -4089,7 +4089,7 @@
         <v>11</v>
       </c>
       <c r="C313" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314">
@@ -4364,7 +4364,7 @@
         <v>4</v>
       </c>
       <c r="C338" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="339">
@@ -4397,7 +4397,7 @@
         <v>7</v>
       </c>
       <c r="C341" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342">
@@ -4496,7 +4496,7 @@
         <v>8</v>
       </c>
       <c r="C350" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="351">
@@ -4672,7 +4672,7 @@
         <v>8</v>
       </c>
       <c r="C366" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367">
@@ -5816,7 +5816,7 @@
         <v>8</v>
       </c>
       <c r="C470" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="471">
@@ -5860,7 +5860,7 @@
         <v>4</v>
       </c>
       <c r="C474" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="475">
@@ -5893,7 +5893,7 @@
         <v>7</v>
       </c>
       <c r="C477" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="478">
@@ -6014,7 +6014,7 @@
         <v>10</v>
       </c>
       <c r="C488" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489">
@@ -6300,7 +6300,7 @@
         <v>4</v>
       </c>
       <c r="C514" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="515">
@@ -6311,7 +6311,7 @@
         <v>5</v>
       </c>
       <c r="C515" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="516">
@@ -6476,7 +6476,7 @@
         <v>4</v>
       </c>
       <c r="C530" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="531">
@@ -6487,7 +6487,7 @@
         <v>5</v>
       </c>
       <c r="C531" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="532">
@@ -6828,7 +6828,7 @@
         <v>4</v>
       </c>
       <c r="C562" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="563">
@@ -6905,7 +6905,7 @@
         <v>11</v>
       </c>
       <c r="C569" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="570">
@@ -6916,7 +6916,7 @@
         <v>4</v>
       </c>
       <c r="C570" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="571">
@@ -6927,7 +6927,7 @@
         <v>5</v>
       </c>
       <c r="C571" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="572">
@@ -7356,7 +7356,7 @@
         <v>4</v>
       </c>
       <c r="C610" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="611">
@@ -7400,7 +7400,7 @@
         <v>8</v>
       </c>
       <c r="C614" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="615">
@@ -7411,7 +7411,7 @@
         <v>9</v>
       </c>
       <c r="C615" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="616">
@@ -7444,7 +7444,7 @@
         <v>4</v>
       </c>
       <c r="C618" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="619">
@@ -7477,7 +7477,7 @@
         <v>7</v>
       </c>
       <c r="C621" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="622">
@@ -8060,7 +8060,7 @@
         <v>4</v>
       </c>
       <c r="C674" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="675">
@@ -8071,7 +8071,7 @@
         <v>5</v>
       </c>
       <c r="C675" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="676">
@@ -8225,7 +8225,7 @@
         <v>11</v>
       </c>
       <c r="C689" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="690">
@@ -8621,7 +8621,7 @@
         <v>7</v>
       </c>
       <c r="C725" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="726">

</xml_diff>